<commit_message>
implement mult-variety basis analyzing
</commit_message>
<xml_diff>
--- a/black_metals/data/mid-stream/螺纹钢/螺纹钢产量.xlsx
+++ b/black_metals/data/mid-stream/螺纹钢/螺纹钢产量.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Projects\ffa\steel\data\mid-stream\螺纹钢\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Projects\futures_nexus\black_metals\data\mid-stream\螺纹钢\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A09CCF-4C73-4B0B-9F6F-3588003B94DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3260646-B691-4487-AF63-FA44DE5AE05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1837" yWindow="2213" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>howard</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DB53ABFD-E16B-43A7-9E78-9FBF0DB5C31B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{98B9CB21-650F-41A4-827F-EEDC58A94FA5}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvM+1uqZaQy5fWsnFn5LuXU8wJ48VaigH4pMxhl3I+UVtddn6UsNbNriJq2tF1otd2Quo8ZTJQifLb7TFDK/wb9m0N2ql9M8X77D45oUHbBxYKhTp/YZ5eg8xC46V0a/9fijMO1qKMzIiTYA4IDYJMyLZkGeuDDYZmt2KehVya8aRUcmVGg7KC1Ap3w1cZSWmPkkgtIbs780EE2lQxSgLT5DPoATQveVWCUigTaU5d9r917VQI1cJ1mdvLduPsDdb0wEUx6NSAfiw6VRYRoxEyHvD9qxAjdIEwgmbV0UjBWqMh0VUPfUsQKiHR8/W38QffkriZyPHDaWOP4SYj/x1mcdu2WTkTbw3y7+d3obAUIpXBvX/k3Micwr3bB7Nbv8n3+VWg3lWkTz+6bnFXJ+xX0iMJx90dO8jEVUrIS/Fdx9XM9O4iAgXOxM58xZWxuzeSbDVHNUUz1mwgS+KODVBsHCUiV6mlm91SOLMlUE1r/1yH697RZXi7RHearzcAa2GSlQcEynFU2dJlbBBW7/aNL/z9amLHBxcI9UPujLO4QY3Cfb4Mz0lFVjNis7TJX/4+RMvtd15bQpIjo+mCMa+7OIe0JJpRjB3TZtaD2iUgMxHRXr96H6NnxfQENkW/GaSpkd1QjElKOUl4Mh3a8Wg4pwdaV8jNI8JQ3vSLbUGYArx5FylWlxPumWldkfDM8V7eNlOkXES6zQvMvlF5KSeY7x3ZIDs8+og7TcQcnOrtjQQglEt4yQKTnXbO4aa3Dm2UMO8e5eSSeuxW0J6yzFlzUSF4GC4YqJ8qnnMz6D/3XB9xDp0EwUM315VQHHqc4zAGiwQiywRiwq4G7f8YfJRjZ0Fy8IanxmN5Ea9zJmy6d5/LZWfx8PvwEeBrGAPCMxZNX/n/wIJMKCyUp1hEKyx3oLpn019N8HfxG3W6VhXXZBskwPvW6UOt4OJITjAmNW7LAPCpEEvaY1yEtDdt4+1sNQPcIhR+MG5Xx3fNGrUS1oBg==</t>
+          <t>yVjpCgZpNvM+1uqZaQy5fWsnFn5LuXU8wJ48VaigH4pMxhl3I+UVtddn6UsNbNriJq2tF1otd2Quo8ZTJQifLb7TFDK/wb9m0N2ql9M8X77D45oUHbBxYKhTp/YZ5eg8xC46V0a/9fijMO1qKMzIiTYA4IDYJMyLZkGeuDDYZmt2KehVya8aRUcmVGg7KC1Ap3w1cZSWmPkkgtIbs780EE2lQxSgLT5DPoATQveVWCUigTaU5d9r917VQI1cJ1mdvLduPsDdb0wEUx6NSAfiw6VRYRoxEyHvD9qxAjdIEwgmbV0UjBWqMh0VUPfUsQKiHR8/W38QffkriZyPHDaWOP4SYj/x1mcdu2WTkTbw3y7+d3obAUIpXBvX/k3Micwr3bB7Nbv8n3+VWg3lWkTz+6bnFXJ+xX0iMJx90dO8jEVUrIS/Fdx9XM9O4iAgXOxM58xZWxuzeSbDVHNUUz1mwgS+KODVBsHCUiV6mlm91SOLMlUE1r/1yH697RZXi7RHearzcAa2GSlQcEynFU2dJlbBBW7/aNL/z9amLHBxcI9UPujLO4QY3Cfb4Mz0lFVjNis7TJX/4+RMvtd15bQpIjo+mCMa+7OIe0JJpRjB3TZtaD2iUgMxHRXr96H6NnxfQENkW/GaSpkd1QjElKOUl4Mh3a8Wg4pwdaV8jNI8JQ3vSLbUGYArx5FylWlxPumWldkfDM8V7eNlOkXES6zQvMvlF5KSeY7x3ZIDs8+og7TcQcnOrtjQQglEt4yQKTnXbO4aa3Dm2UMO8e5eSSeuxW0J6yzFlzUSF4GC4YqJ8qnnMz6D/3XB9xDp0EwUM315VQHHqc4zAGiwQiywRiwq4G7f8YfJRjZ0Fy8IanxmN5Ea9zJmy6d5/G2pogyS5Qgw7PCJXLVcTtx91vS0UGZ7u/bIESRiESD/4bme/c/RwWCXwoV9BAKAyyexhrh6Cf9/7LuuCE4wQSdvmAlV2VuPRUY7cc6IWvKnV1kinMIYX45m2c6N+aJVwQ==</t>
         </r>
       </text>
     </comment>
@@ -111,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,14 +155,6 @@
       <b/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -237,7 +229,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -258,9 +250,6 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,10 +751,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3442,18 +3431,31 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="5">
+        <v>45351</v>
+      </c>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6">
+        <v>3209.9</v>
+      </c>
+      <c r="E161" s="6">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>